<commit_message>
new pathologyID column name in metadata, updated README
</commit_message>
<xml_diff>
--- a/Documentation/pathologies.xlsx
+++ b/Documentation/pathologies.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t xml:space="preserve">Acronym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compatibility groups</t>
+    <t xml:space="preserve">pathologyID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compatibility groups</t>
   </si>
   <si>
     <t xml:space="preserve">MMAF</t>
@@ -223,13 +223,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>